<commit_message>
Se añaden respaldos y datos duplicados
</commit_message>
<xml_diff>
--- a/app/common/data/students_cleaned.xlsx
+++ b/app/common/data/students_cleaned.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R706"/>
+  <dimension ref="A1:R708"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44235,6 +44235,130 @@
         <v>61</v>
       </c>
     </row>
+    <row r="707">
+      <c r="A707" t="n">
+        <v>710</v>
+      </c>
+      <c r="B707" t="n">
+        <v>18</v>
+      </c>
+      <c r="C707" t="n">
+        <v>1</v>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="F707" t="n">
+        <v>5</v>
+      </c>
+      <c r="G707" t="inlineStr">
+        <is>
+          <t>YouTube</t>
+        </is>
+      </c>
+      <c r="H707" t="n">
+        <v>1</v>
+      </c>
+      <c r="I707" t="n">
+        <v>7</v>
+      </c>
+      <c r="J707" t="n">
+        <v>7</v>
+      </c>
+      <c r="K707" t="n">
+        <v>1</v>
+      </c>
+      <c r="L707" t="n">
+        <v>1</v>
+      </c>
+      <c r="M707" t="n">
+        <v>10</v>
+      </c>
+      <c r="N707" t="n">
+        <v>0</v>
+      </c>
+      <c r="O707" t="n">
+        <v>0</v>
+      </c>
+      <c r="P707" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q707" t="n">
+        <v>4</v>
+      </c>
+      <c r="R707" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="n">
+        <v>706</v>
+      </c>
+      <c r="B708" t="n">
+        <v>18</v>
+      </c>
+      <c r="C708" t="n">
+        <v>1</v>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>High School</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="F708" t="n">
+        <v>5</v>
+      </c>
+      <c r="G708" t="inlineStr">
+        <is>
+          <t>YouTube</t>
+        </is>
+      </c>
+      <c r="H708" t="n">
+        <v>1</v>
+      </c>
+      <c r="I708" t="n">
+        <v>7</v>
+      </c>
+      <c r="J708" t="n">
+        <v>7</v>
+      </c>
+      <c r="K708" t="n">
+        <v>1</v>
+      </c>
+      <c r="L708" t="n">
+        <v>1</v>
+      </c>
+      <c r="M708" t="n">
+        <v>10</v>
+      </c>
+      <c r="N708" t="n">
+        <v>0</v>
+      </c>
+      <c r="O708" t="n">
+        <v>0</v>
+      </c>
+      <c r="P708" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q708" t="n">
+        <v>4</v>
+      </c>
+      <c r="R708" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>